<commit_message>
Ajout Dico de Données pour exos du jour
</commit_message>
<xml_diff>
--- a/Exercices/01 - Concevoir une base de données/01 - Concevoir une base de données/00 - Entrainements/1 Exercices_Merise/04 - Bibliothèque/04 - Dictionnaire de Données.xlsx
+++ b/Exercices/01 - Concevoir une base de données/01 - Concevoir une base de données/00 - Entrainements/1 Exercices_Merise/04 - Bibliothèque/04 - Dictionnaire de Données.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25726"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C49CA0F1-1DCB-4690-82CB-C86D90F417E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="-12090" yWindow="2880" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -16,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="64">
   <si>
     <t>Nom</t>
   </si>
@@ -43,13 +44,178 @@
   </si>
   <si>
     <t>Exemplaire</t>
+  </si>
+  <si>
+    <t>Identifiant exemplaire</t>
+  </si>
+  <si>
+    <t>Auteurs</t>
+  </si>
+  <si>
+    <t>Identifiant de l'auteur</t>
+  </si>
+  <si>
+    <t>Nom de l'auteur</t>
+  </si>
+  <si>
+    <t>Prénom de l'auteur</t>
+  </si>
+  <si>
+    <t>Rayons</t>
+  </si>
+  <si>
+    <t>Identifiant du rayon</t>
+  </si>
+  <si>
+    <t>Nom du rayon</t>
+  </si>
+  <si>
+    <t>Mots clès</t>
+  </si>
+  <si>
+    <t>Identifiant du mot clès</t>
+  </si>
+  <si>
+    <t>Mot clès</t>
+  </si>
+  <si>
+    <t>Adhérents</t>
+  </si>
+  <si>
+    <t>Identifiant de l'Adhérent</t>
+  </si>
+  <si>
+    <t>Nom de l'adhérent</t>
+  </si>
+  <si>
+    <t>Prénom de l'adhérent</t>
+  </si>
+  <si>
+    <t>Identifiant de la bibliothèque</t>
+  </si>
+  <si>
+    <t>Bibliothèques</t>
+  </si>
+  <si>
+    <t>Nom de la bibliothèque</t>
+  </si>
+  <si>
+    <t>Fonds de la bibliothèque</t>
+  </si>
+  <si>
+    <t>Centrale ou antenne</t>
+  </si>
+  <si>
+    <t>Emprunts</t>
+  </si>
+  <si>
+    <t>Date de l'emprunt</t>
+  </si>
+  <si>
+    <t>Date de retour prévu</t>
+  </si>
+  <si>
+    <t>État de l'exemplaire (extra)</t>
+  </si>
+  <si>
+    <t>dateEmprunt</t>
+  </si>
+  <si>
+    <t>dateRetourPrevu</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>NN</t>
+  </si>
+  <si>
+    <t>PK=&gt;PrimaryKey</t>
+  </si>
+  <si>
+    <t>NN=&gt; Not Null</t>
+  </si>
+  <si>
+    <t>Bool</t>
+  </si>
+  <si>
+    <t>centrale</t>
+  </si>
+  <si>
+    <t>default=false</t>
+  </si>
+  <si>
+    <t>fondsBibliotheque</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>nomBibliotheque</t>
+  </si>
+  <si>
+    <t>Varchar</t>
+  </si>
+  <si>
+    <t>idBibliotheque</t>
+  </si>
+  <si>
+    <t>Compteur</t>
+  </si>
+  <si>
+    <t>PK</t>
+  </si>
+  <si>
+    <t>prenomAdherent</t>
+  </si>
+  <si>
+    <t>nomAdherent</t>
+  </si>
+  <si>
+    <t>idAdherent</t>
+  </si>
+  <si>
+    <t>motCles</t>
+  </si>
+  <si>
+    <t>idMotCles</t>
+  </si>
+  <si>
+    <t>idRayon</t>
+  </si>
+  <si>
+    <t>nomRayon</t>
+  </si>
+  <si>
+    <t>prenomAuteur</t>
+  </si>
+  <si>
+    <t>nomAuteur</t>
+  </si>
+  <si>
+    <t>idAuteur</t>
+  </si>
+  <si>
+    <t>etatExemplaire</t>
+  </si>
+  <si>
+    <t>idExemplaire</t>
+  </si>
+  <si>
+    <t>codeISBN</t>
+  </si>
+  <si>
+    <t>titreOuvrage</t>
+  </si>
+  <si>
+    <t>idOuvrage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -70,8 +236,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -81,6 +254,54 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -170,11 +391,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -188,43 +417,79 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="6" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="6" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="6" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="10">
+    <cellStyle name="20 % - Accent1" xfId="2" builtinId="30"/>
+    <cellStyle name="40 % - Accent1" xfId="3" builtinId="31"/>
+    <cellStyle name="40 % - Accent2" xfId="4" builtinId="35"/>
     <cellStyle name="60 % - Accent1" xfId="1" builtinId="32"/>
+    <cellStyle name="60 % - Accent2" xfId="5" builtinId="36"/>
+    <cellStyle name="60 % - Accent3" xfId="6" builtinId="40"/>
+    <cellStyle name="60 % - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="60 % - Accent5" xfId="8" builtinId="48"/>
+    <cellStyle name="60 % - Accent6" xfId="9" builtinId="52"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -323,13 +588,6 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -347,6 +605,32 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -362,13 +646,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:D24" totalsRowShown="0" headerRowDxfId="0" dataDxfId="8" headerRowBorderDxfId="6" tableBorderDxfId="7" totalsRowBorderDxfId="5">
-  <autoFilter ref="A1:D24"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="A1:D30" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+  <autoFilter ref="A1:D30" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Nom" dataDxfId="4"/>
-    <tableColumn id="2" name="Libellé" dataDxfId="3"/>
-    <tableColumn id="3" name="Type" dataDxfId="2"/>
-    <tableColumn id="4" name="Code" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Nom" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Libellé" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Type" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Code" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -450,6 +734,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -485,6 +786,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -660,17 +978,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" customWidth="1"/>
+    <col min="1" max="1" width="37" customWidth="1"/>
     <col min="2" max="2" width="36.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
     <col min="4" max="4" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -697,25 +1016,43 @@
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
+      <c r="B3" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
+      <c r="B4" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
+      <c r="B5" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -723,112 +1060,345 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
+      <c r="A7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
+      <c r="A8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
+      <c r="A9" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
+      <c r="A10" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
+      <c r="A11" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
+      <c r="A12" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
+      <c r="A13" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
+      <c r="A14" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
+      <c r="A15" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+    </row>
+    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="D25" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D27" s="19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="D29" s="23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="D30" s="25" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="20"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="20"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="20"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="20"/>
+      <c r="B34" s="20"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="21"/>
+      <c r="B35" s="21"/>
+      <c r="C35" s="21"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -839,7 +1409,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -851,7 +1421,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>